<commit_message>
File Upload Concept Covered
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/gorest/testdata/GoRestTestData.xlsx
+++ b/src/main/java/com/qa/gorest/testdata/GoRestTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHUTOSH SINGH\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHUTOSH SINGH\eclipse-workspace\RestAssuredAug2\src\main\java\com\qa\gorest\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7B42C70-C27E-407A-A212-6EA66149CC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAE9258-781D-4ECE-A258-972A56AF8951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D1008E38-9F31-4729-B83F-58C76617339A}"/>
   </bookViews>
@@ -59,18 +59,6 @@
     <t>manoj</t>
   </si>
   <si>
-    <t>priya@msn.usa</t>
-  </si>
-  <si>
-    <t>neha008b@gmail.com</t>
-  </si>
-  <si>
-    <t>peeyush@yahoo.india</t>
-  </si>
-  <si>
-    <t>manoj_verma.hotmail@yahoo.g.india</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -86,25 +74,37 @@
     <t>pallavi</t>
   </si>
   <si>
-    <t>pallavi.india@ac.india.in</t>
-  </si>
-  <si>
     <t>Sampath</t>
   </si>
   <si>
-    <t>Sampath@hotmail.india.us</t>
-  </si>
-  <si>
     <t>ramesh</t>
   </si>
   <si>
-    <t>ramesh.rai123@google.india</t>
-  </si>
-  <si>
     <t>aditya</t>
   </si>
   <si>
     <t>aditya@yahoo.us.in</t>
+  </si>
+  <si>
+    <t>priya@msn.usa123</t>
+  </si>
+  <si>
+    <t>neha008b@12gmail.com</t>
+  </si>
+  <si>
+    <t>peeyush@yah12oo.india</t>
+  </si>
+  <si>
+    <t>pallavi.india@ac.indiaa.in</t>
+  </si>
+  <si>
+    <t>Sampath@hotmail.ind1.us</t>
+  </si>
+  <si>
+    <t>ramesh.r123g@google.india</t>
+  </si>
+  <si>
+    <t>manoj_verma@yahoo.g12.india</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,13 +528,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -542,13 +542,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,13 +556,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -570,69 +570,69 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allure Report Plugins added
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/gorest/testdata/GoRestTestData.xlsx
+++ b/src/main/java/com/qa/gorest/testdata/GoRestTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASHUTOSH SINGH\eclipse-workspace\RestAssuredAug2\src\main\java\com\qa\gorest\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944C9640-75A5-4EDA-B4FB-67FDC9EA7331}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BD74DD-49FA-40EE-AE25-E41A0131D490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D1008E38-9F31-4729-B83F-58C76617339A}"/>
   </bookViews>
@@ -83,28 +83,28 @@
     <t>Amit</t>
   </si>
   <si>
-    <t>priya@msn2.usa123</t>
-  </si>
-  <si>
-    <t>neha008in@12gmail.com</t>
-  </si>
-  <si>
-    <t>peeyush12@yah12oo.india</t>
-  </si>
-  <si>
-    <t>manoj_verma34@yahoo.g12.india</t>
-  </si>
-  <si>
-    <t>pallavi_india24@ac.indiaa.in</t>
-  </si>
-  <si>
-    <t>Sampath@hotmail.in1.us</t>
-  </si>
-  <si>
-    <t>ramesh.r123h@google.in.uk</t>
-  </si>
-  <si>
-    <t>aditya12@yahoo.au.in</t>
+    <t>priya6u@msn2.usa123</t>
+  </si>
+  <si>
+    <t>neha6u8in@12gmail.com</t>
+  </si>
+  <si>
+    <t>peeyush16u2@yah12oo.india</t>
+  </si>
+  <si>
+    <t>manoj_verma6u34@yahoo.g12.india</t>
+  </si>
+  <si>
+    <t>pallavi_india26u4@ac.indiaa.in</t>
+  </si>
+  <si>
+    <t>Sampath@hotma6uil.in1.us</t>
+  </si>
+  <si>
+    <t>ramesh.r1236uh@google.in.uk</t>
+  </si>
+  <si>
+    <t>aditya126u@yahoo.au.in</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,16 +636,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5E7D221A-31F9-4FE0-AD16-AB21C0ECD659}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{CC60D9B8-E7E3-4A41-9BEE-F2795D1330A3}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{D1561C77-24B0-4EDA-8450-22235DCA3E00}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{276A9979-BEE2-40A4-A751-8290ECD14DE9}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{E7F1CFE0-B805-4525-A3B2-5152176F5B4F}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{A6A96D83-0FBA-4B54-9676-2B53E5C9655E}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{1AAE117F-CC4A-440E-BEEA-9237AF0622DA}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{D44286A9-09F9-49E9-8F62-D6698C02B008}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>